<commit_message>
Changes to scr files for opensource version of the model
</commit_message>
<xml_diff>
--- a/project_example/01_external_data/scenarios/sets/aggregation/Years_interpolation.xlsx
+++ b/project_example/01_external_data/scenarios/sets/aggregation/Years_interpolation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boonmanhj\Documents\Gitlab\tno-eco-mod-ci\project_open_entrance\01_external_data\scenarios\sets\aggregation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boonmanhj\Documents\Gitlab\tno-eco-mod-ci\project_example\01_external_data\scenarios\sets\aggregation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E8A992-BACF-4661-A0A8-8529BA57ABBD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CAAF71-08E7-460C-AA90-8A92F5BA536A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Years_interpolation1" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="64">
   <si>
     <t>yr2010</t>
   </si>
@@ -191,6 +191,36 @@
   </si>
   <si>
     <t>YR2050</t>
+  </si>
+  <si>
+    <t>year2007</t>
+  </si>
+  <si>
+    <t>year2010</t>
+  </si>
+  <si>
+    <t>year2015</t>
+  </si>
+  <si>
+    <t>year2020</t>
+  </si>
+  <si>
+    <t>year2025</t>
+  </si>
+  <si>
+    <t>year2030</t>
+  </si>
+  <si>
+    <t>year2035</t>
+  </si>
+  <si>
+    <t>year2040</t>
+  </si>
+  <si>
+    <t>year2045</t>
+  </si>
+  <si>
+    <t>year2050</t>
   </si>
 </sst>
 </file>
@@ -574,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4906F231-CD2B-436D-9BC7-9C357742E490}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,35 +643,35 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>6</v>
-      </c>
-      <c r="H2">
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <v>8</v>
-      </c>
-      <c r="J2">
-        <v>9</v>
-      </c>
-      <c r="K2">
-        <v>10</v>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -976,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7337CF6-33DB-4BA9-9AE9-F2F8B2DF101F}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,35 +1045,35 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>6</v>
-      </c>
-      <c r="H2">
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <v>8</v>
-      </c>
-      <c r="J2">
-        <v>9</v>
-      </c>
-      <c r="K2">
-        <v>10</v>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1399,6 +1429,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>